<commit_message>
Added reading base nodes (v0.1.4)
* Added the functions that read the base nodes from an Excel file.
* Added basic unit tests to validate these functions.
</commit_message>
<xml_diff>
--- a/test/base/baseConfig.xlsx
+++ b/test/base/baseConfig.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Attributes" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Nodes" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Base Nodes" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Compound Nodes" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Transition types" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="IN Transitions" sheetId="6" state="visible" r:id="rId7"/>
@@ -1149,7 +1149,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1648,7 +1648,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:B19" type="list">
-      <formula1>OFFSET(Nodes!$A$7,0,0,Nodes!$B$4)</formula1>
+      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1931,7 +1931,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C12:D21" type="list">
-      <formula1>OFFSET(Nodes!$A$7,0,0,Nodes!$B$4)</formula1>
+      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2619,7 +2619,7 @@
   <dimension ref="A1:K1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21299,7 +21299,7 @@
   <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21376,7 +21376,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AMI7" s="1"/>
       <c r="AMJ7" s="1"/>
@@ -21404,7 +21404,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21434,7 +21434,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21448,9 +21448,7 @@
         <f aca="true">MATCH($A12,OFFSET(INDIRECT(CONCATENATE(Misc!$A$7,"A2")),0,0,INDIRECT(CONCATENATE(Misc!$A$5,"B6")),1),0)</f>
         <v>6</v>
       </c>
-      <c r="D12" s="12" t="n">
-        <v>1</v>
-      </c>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16"/>
@@ -22911,7 +22909,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8 G8 L8" type="list">
-      <formula1>OFFSET(Nodes!$A$7,0,0,Nodes!$B$4)</formula1>
+      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9:B10 G9:G10 L9:L10" type="decimal">
@@ -23853,7 +23851,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C7 B11:C11 B15:C15 B19:C19 B23:C23 B27:C27" type="list">
-      <formula1>OFFSET(Nodes!$A$7,0,0,Nodes!$B$4)</formula1>
+      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:H6 A8:C8 G8:G10 A9 C9 H10 A12:C12 G12:G14 A13 C13 H14 A16:C16 G16:G18 A17 C17 H18 A20:C20 G20:G22 A21 C21 H22 A24:C24 G24:G26 A25 C25 H26 A28:C28 G28:G29 A29 C29" type="none">
@@ -29796,7 +29794,7 @@
   </conditionalFormatting>
   <dataValidations count="15">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7" type="list">
-      <formula1>OFFSET(Nodes!$A$7,0,0,Nodes!$B$4)</formula1>
+      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
@@ -29804,7 +29802,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11 B15 B19 B23 B27" type="list">
-      <formula1>OFFSET(Nodes!$A$7,0,0,Nodes!$B$4)</formula1>
+      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:G6 A8:B8 F8:F10 A9 G10 A12:B12 F12:F14 A13 G14 A16:B16 F16:F18 A17 G18 A20:B20 F20:F22 A21 G22 A24:B24 F24:F26 A25 G26 A28:B28 F28:F29 A29" type="none">

</xml_diff>

<commit_message>
Added reading compound nodes (v0.1.5)
* Added the functions that read the base nodes from an Excel file.
* Added basic unit tests to validate these functions
</commit_message>
<xml_diff>
--- a/test/base/baseConfig.xlsx
+++ b/test/base/baseConfig.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="202">
   <si>
     <t xml:space="preserve">General simulation parameters</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t xml:space="preserve">Component nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch A</t>
   </si>
   <si>
     <t xml:space="preserve">Transition types</t>
@@ -1309,7 +1315,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1317,7 +1323,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>12</v>
@@ -1325,15 +1331,15 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>1</v>
@@ -1341,7 +1347,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>7</v>
@@ -1349,7 +1355,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>15</v>
@@ -1357,7 +1363,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>6</v>
@@ -1365,7 +1371,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>15</v>
@@ -1373,7 +1379,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>8</v>
@@ -1385,7 +1391,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B12" s="12" t="n">
         <v>100</v>
@@ -1397,7 +1403,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B13" s="14" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B13,3,-1,B12)),0,0),0)-1,B12)</f>
@@ -1410,7 +1416,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>51</v>
@@ -1421,7 +1427,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,7 +1435,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1437,7 +1443,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,7 +1451,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,7 +1517,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -1521,7 +1527,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>12</v>
@@ -1529,7 +1535,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>25</v>
@@ -1537,7 +1543,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>12</v>
@@ -1545,10 +1551,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1557,7 +1563,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B8" s="12" t="n">
         <v>1000</v>
@@ -1569,7 +1575,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B9" s="17" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B9,2,0,B8)),0,0),0)-1,B8)</f>
@@ -1582,25 +1588,25 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,6 +1637,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:B19" type="list">
+      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B5" type="list">
       <formula1>Misc!$B$1:$B$2</formula1>
       <formula2>0</formula2>
@@ -1645,10 +1655,6 @@
     </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4" type="list">
       <formula1>Misc!$E$1:$E$4</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:B19" type="list">
-      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1688,7 +1694,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B1" s="40"/>
     </row>
@@ -1698,7 +1704,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>12</v>
@@ -1706,7 +1712,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>12</v>
@@ -1714,7 +1720,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>12</v>
@@ -1722,10 +1728,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,7 +1740,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B8" s="12" t="n">
         <v>50</v>
@@ -1746,7 +1752,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B9" s="14" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B9,3,3,B8)),0,0),0)-1,B8)</f>
@@ -1759,19 +1765,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,10 +1786,10 @@
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E12" s="18"/>
     </row>
@@ -1793,10 +1799,10 @@
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E13" s="18"/>
     </row>
@@ -1806,7 +1812,7 @@
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>42</v>
@@ -1819,7 +1825,7 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>42</v>
@@ -1832,7 +1838,7 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="18"/>
@@ -1843,7 +1849,7 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="18"/>
@@ -1854,7 +1860,7 @@
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="18"/>
@@ -1865,7 +1871,7 @@
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="18"/>
@@ -1973,7 +1979,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B1" s="40"/>
     </row>
@@ -1983,7 +1989,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>12</v>
@@ -1991,7 +1997,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>12</v>
@@ -1999,7 +2005,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>12</v>
@@ -2007,10 +2013,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,7 +2025,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B8" s="12" t="n">
         <v>50</v>
@@ -2031,7 +2037,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B9" s="14" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B9,4,0,B8)),0,0),0)-1,B8)</f>
@@ -2056,32 +2062,32 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,7 +2117,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="36" t="s">
@@ -2138,7 +2144,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="36" t="s">
@@ -2165,7 +2171,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="36" t="s">
@@ -2192,7 +2198,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="36" t="s">
@@ -2219,7 +2225,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="36" t="s">
@@ -2246,7 +2252,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="36" t="s">
@@ -2273,7 +2279,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="36" t="s">
@@ -2300,7 +2306,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="36" t="s">
@@ -2327,7 +2333,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="36" t="s">
@@ -2381,7 +2387,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="36" t="s">
@@ -2435,7 +2441,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="36" t="s">
@@ -2462,7 +2468,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="36" t="s">
@@ -2489,7 +2495,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="36" t="s">
@@ -2516,7 +2522,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="36" t="s">
@@ -2543,7 +2549,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="36" t="s">
@@ -2638,19 +2644,19 @@
         <v>15</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H1" s="41" t="n">
         <f aca="false">ROWS(H2:H1001)-COUNTIF(H2:H1001,"")</f>
@@ -2665,7 +2671,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="41" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,19 +2683,19 @@
         <v>12</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H2" s="43" t="str">
         <f aca="true" t="array" ref="H2:H2">IFERROR(INDEX(OFFSET('Transition types'!$A$6,1,0,'Transition types'!$B$4),SMALL(IF(OFFSET('Transition types'!$C$6,1,0,'Transition types'!$B$4)="IN",OFFSET($K$2,0,0,'Transition types'!$B$4)),ROWS($K$2:$K2))),"")</f>
@@ -2714,19 +2720,19 @@
         <v>.</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H3" s="43" t="str">
         <f aca="true" t="array" ref="H3:H3">IFERROR(INDEX(OFFSET('Transition types'!$A$6,1,0,'Transition types'!$B$4),SMALL(IF(OFFSET('Transition types'!$C$6,1,0,'Transition types'!$B$4)="IN",OFFSET($K$2,0,0,'Transition types'!$B$4)),ROWS($K$2:$K3))),"")</f>
@@ -2751,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E4" s="41" t="s">
         <v>25</v>
@@ -2779,7 +2785,7 @@
         <v>'catalogue.xlsx'#'General'.</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H5" s="43" t="str">
         <f aca="true" t="array" ref="H5:H5">IFERROR(INDEX(OFFSET('Transition types'!$A$6,1,0,'Transition types'!$B$4),SMALL(IF(OFFSET('Transition types'!$C$6,1,0,'Transition types'!$B$4)="IN",OFFSET($K$2,0,0,'Transition types'!$B$4)),ROWS($K$2:$K5))),"")</f>
@@ -2804,7 +2810,7 @@
         <v>'catalogue.xlsx'#'Attributes'.</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H6" s="43" t="str">
         <f aca="true" t="array" ref="H6:H6">IFERROR(INDEX(OFFSET('Transition types'!$A$6,1,0,'Transition types'!$B$4),SMALL(IF(OFFSET('Transition types'!$C$6,1,0,'Transition types'!$B$4)="IN",OFFSET($K$2,0,0,'Transition types'!$B$4)),ROWS($K$2:$K6))),"")</f>
@@ -2829,7 +2835,7 @@
         <v>'catalogue.xlsx'#'States'.</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H7" s="43" t="str">
         <f aca="true" t="array" ref="H7:H7">IFERROR(INDEX(OFFSET('Transition types'!$A$6,1,0,'Transition types'!$B$4),SMALL(IF(OFFSET('Transition types'!$C$6,1,0,'Transition types'!$B$4)="IN",OFFSET($K$2,0,0,'Transition types'!$B$4)),ROWS($K$2:$K7))),"")</f>
@@ -2854,7 +2860,7 @@
         <v>'catalogue.xlsx'#'Transition types'.</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H8" s="43" t="str">
         <f aca="true" t="array" ref="H8:H8">IFERROR(INDEX(OFFSET('Transition types'!$A$6,1,0,'Transition types'!$B$4),SMALL(IF(OFFSET('Transition types'!$C$6,1,0,'Transition types'!$B$4)="IN",OFFSET($K$2,0,0,'Transition types'!$B$4)),ROWS($K$2:$K8))),"")</f>
@@ -21298,7 +21304,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -21530,8 +21536,8 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21598,21 +21604,21 @@
       </c>
       <c r="B4" s="14" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B4,3,-1,B3)),0,0),0)-1,B3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>48</v>
       </c>
       <c r="F4" s="14" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(F4,3,-1,F3)),0,0),0)-1,F3)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>49</v>
       </c>
       <c r="I4" s="14" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(I4,3,-1,I3)),0,0),0)-1,I3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21654,19 +21660,29 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16"/>
-      <c r="C7" s="17" t="e">
+      <c r="A7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="17" t="n">
         <f aca="true">MATCH($A7,OFFSET(INDIRECT(CONCATENATE(Misc!$A$7,"A2")),0,0,INDIRECT(CONCATENATE(Misc!$A$5,"B6")),1),0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="H7" s="16"/>
+        <v>9</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="J7" s="17" t="n">
         <f aca="true">MATCH(TRUE(),INDEX(ISBLANK(OFFSET(J7,0,1,1,200)),0,0),0)-1</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+        <v>2</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
     </row>
@@ -21676,7 +21692,9 @@
         <f aca="true">MATCH($A8,OFFSET(INDIRECT(CONCATENATE(Misc!$A$7,"A2")),0,0,INDIRECT(CONCATENATE(Misc!$A$5,"B6")),1),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="H8" s="16"/>
       <c r="J8" s="17" t="n">
         <f aca="true">MATCH(TRUE(),INDEX(ISBLANK(OFFSET(J8,0,1,1,200)),0,0),0)-1</f>
@@ -21795,12 +21813,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" s="12" t="n">
         <v>1000</v>
@@ -21808,7 +21826,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B4" s="14" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B4,3,-1,B3)),0,0),0)-1,B3)</f>
@@ -21817,18 +21835,18 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B7" s="12" t="n">
         <v>5</v>
@@ -21840,7 +21858,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B8" s="12" t="n">
         <v>3</v>
@@ -21852,7 +21870,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B9" s="12" t="n">
         <v>2</v>
@@ -21864,7 +21882,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B10" s="12" t="n">
         <v>4</v>
@@ -21876,7 +21894,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B11" s="12" t="n">
         <v>1</v>
@@ -22018,7 +22036,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -22028,7 +22046,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>3</v>
@@ -22040,97 +22058,97 @@
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G6" s="6" t="n">
         <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L6" s="6" t="n">
         <v>12</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L7" s="6" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>39</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>38</v>
@@ -22145,7 +22163,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -22157,7 +22175,7 @@
         <v>40</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I9" s="11"/>
       <c r="K9" s="23" t="str">
@@ -22168,7 +22186,7 @@
         <v>40</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N9" s="11"/>
     </row>
@@ -22181,7 +22199,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -22193,7 +22211,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I10" s="11"/>
       <c r="K10" s="23" t="str">
@@ -22204,25 +22222,25 @@
         <v>10</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="K11" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>12</v>
@@ -22253,19 +22271,19 @@
     </row>
     <row r="13" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K13" s="23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>15</v>
@@ -22280,7 +22298,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -22292,7 +22310,7 @@
         <v>20</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I14" s="11"/>
       <c r="K14" s="23" t="str">
@@ -22303,7 +22321,7 @@
         <v>20</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="N14" s="11"/>
     </row>
@@ -22318,7 +22336,7 @@
         <v>ignored</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -22328,7 +22346,7 @@
         <v>ignored</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -22337,7 +22355,7 @@
         <v>ignored</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
@@ -22352,7 +22370,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D17" s="25" t="n">
         <f aca="true">SUMIF(OFFSET(D17,2,-1,B17),"&gt; 0")</f>
@@ -22368,7 +22386,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I17" s="27" t="n">
         <f aca="true">SUMIF(OFFSET(I17,2,-1,G17),"&gt; 0")</f>
@@ -22383,7 +22401,7 @@
         <v>4</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="N17" s="27" t="n">
         <f aca="true">SUMIF(OFFSET(N17,2,-1,L17),"&gt; 0")</f>
@@ -22392,13 +22410,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D18" s="9" t="str">
         <f aca="false">IF(B16="Pointwise","Normalised","")</f>
@@ -22406,26 +22424,26 @@
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I18" s="28" t="str">
         <f aca="false">IF(G16="Pointwise","Normalised","")</f>
         <v/>
       </c>
       <c r="K18" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N18" s="28" t="str">
         <f aca="false">IF(L16="Pointwise","Normalised","")</f>
@@ -22570,7 +22588,7 @@
         <v>ignored</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C24" s="11"/>
       <c r="F24" s="23" t="str">
@@ -22578,7 +22596,7 @@
         <v>ignored</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H24" s="11"/>
       <c r="K24" s="23" t="str">
@@ -22586,7 +22604,7 @@
         <v>ignored</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M24" s="11"/>
     </row>
@@ -22600,7 +22618,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D25" s="25" t="n">
         <f aca="true">SUMIF(OFFSET(D25,2,-1,B25),"&gt; 0")</f>
@@ -22616,7 +22634,7 @@
         <v>3</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I25" s="27" t="n">
         <f aca="true">SUMIF(OFFSET(I25,2,-1,G25),"&gt; 0")</f>
@@ -22631,7 +22649,7 @@
         <v>3</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="N25" s="27" t="n">
         <f aca="true">SUMIF(OFFSET(N25,2,-1,L25),"&gt; 0")</f>
@@ -22640,13 +22658,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D26" s="3" t="str">
         <f aca="false">IF(B24="Pointwise","Normalised","")</f>
@@ -22654,26 +22672,26 @@
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I26" s="1" t="str">
         <f aca="false">IF(G24="Pointwise","Normalised","")</f>
         <v>Normalised</v>
       </c>
       <c r="K26" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N26" s="1" t="str">
         <f aca="false">IF(L24="Pointwise","Normalised","")</f>
@@ -22980,7 +22998,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -22990,7 +23008,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="12" t="n">
         <v>1000</v>
@@ -23002,7 +23020,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" s="30" t="n">
         <f aca="true">COUNTA(OFFSET(A6,0,0,B3*4)) - COUNTIF(OFFSET(A6,0,0,B3*4), "=Name")</f>
@@ -23018,58 +23036,58 @@
         <v>19</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K6" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L6" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M6" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N6" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O6" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="P6" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Q6" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="S6" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T6" s="31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AME6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>37</v>
@@ -23088,7 +23106,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J7" s="27" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(J8,0,1,1,200)),0,0),0)-1,200)</f>
@@ -23125,7 +23143,7 @@
       <c r="C8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K8" s="12"/>
       <c r="T8" s="12"/>
@@ -23147,58 +23165,58 @@
         <v>19</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K10" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M10" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O10" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="P10" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Q10" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="S10" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T10" s="31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AME10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>39</v>
@@ -23217,7 +23235,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J11" s="27" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(J12,0,1,1,200)),0,0),0)-1,200)</f>
@@ -23254,7 +23272,7 @@
       <c r="C12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K12" s="12"/>
       <c r="T12" s="12"/>
@@ -23276,59 +23294,59 @@
         <v>19</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K14" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L14" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N14" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="P14" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Q14" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="S14" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T14" s="31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AME14" s="1"/>
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>40</v>
@@ -23347,7 +23365,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J15" s="27" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(J16,0,1,1,200)),0,0),0)-1,200)</f>
@@ -23385,7 +23403,7 @@
       <c r="C16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K16" s="12"/>
       <c r="T16" s="12"/>
@@ -23409,59 +23427,59 @@
         <v>19</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K18" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L18" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M18" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N18" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O18" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="P18" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Q18" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="S18" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T18" s="31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AME18" s="1"/>
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>41</v>
@@ -23480,7 +23498,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J19" s="27" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(J20,0,1,1,200)),0,0),0)-1,200)</f>
@@ -23518,7 +23536,7 @@
       <c r="C20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K20" s="12"/>
       <c r="T20" s="12"/>
@@ -23542,59 +23560,59 @@
         <v>19</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H22" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J22" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K22" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L22" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M22" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N22" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O22" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="P22" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Q22" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="S22" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T22" s="31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AME22" s="1"/>
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>38</v>
@@ -23613,7 +23631,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J23" s="27" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(J24,0,1,1,200)),0,0),0)-1,200)</f>
@@ -23651,7 +23669,7 @@
       <c r="C24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K24" s="12"/>
       <c r="T24" s="12"/>
@@ -23675,59 +23693,59 @@
         <v>19</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J26" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K26" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L26" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N26" s="31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O26" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="P26" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Q26" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="S26" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T26" s="31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AME26" s="1"/>
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>38</v>
@@ -23746,7 +23764,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J27" s="27" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(J28,0,1,1,200)),0,0),0)-1,200)</f>
@@ -23784,7 +23802,7 @@
       <c r="C28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K28" s="12"/>
       <c r="T28" s="12"/>
@@ -23951,7 +23969,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="0"/>
@@ -26005,7 +26023,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B3" s="12" t="n">
         <v>1000</v>
@@ -27035,7 +27053,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" s="30" t="n">
         <f aca="true">COUNTA(OFFSET(A6,0,0,B3*4)) - COUNTIF(OFFSET(A6,0,0,B3*4), "=Name")</f>
@@ -29095,47 +29113,47 @@
         <v>19</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K6" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L6" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M6" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N6" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O6" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>37</v>
@@ -29152,7 +29170,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="27" t="n">
@@ -29178,7 +29196,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="G8" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -29210,47 +29228,47 @@
         <v>19</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K10" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M10" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O10" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>39</v>
@@ -29267,7 +29285,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="27" t="n">
@@ -29293,7 +29311,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="G12" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -29325,47 +29343,47 @@
         <v>19</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K14" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L14" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N14" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>38</v>
@@ -29382,7 +29400,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="27" t="n">
@@ -29408,7 +29426,7 @@
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="G16" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -29440,47 +29458,47 @@
         <v>19</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K18" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L18" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M18" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N18" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O18" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>40</v>
@@ -29497,7 +29515,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="27" t="n">
@@ -29523,7 +29541,7 @@
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="G20" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
@@ -29555,47 +29573,47 @@
         <v>19</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J22" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K22" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L22" s="31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M22" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N22" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O22" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>41</v>
@@ -29612,7 +29630,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="27" t="n">
@@ -29638,7 +29656,7 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="G24" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -29670,47 +29688,47 @@
         <v>19</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="35" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J26" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L26" s="35" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M26" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N26" s="35" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O26" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>42</v>
@@ -29727,7 +29745,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="25" t="n">
@@ -29753,7 +29771,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="G28" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
@@ -29883,7 +29901,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -29893,57 +29911,57 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added reading default retirement (v0.1.7)
* Added the functions that read the fallback retirement scheme from an Excel file.
* Added basic unit tests to validate these functions.
</commit_message>
<xml_diff>
--- a/test/base/baseConfig.xlsx
+++ b/test/base/baseConfig.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
     <sheet name="IN Transitions" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="THROUGH Transitions" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="OUT Transitions" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Retirement test" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Default retirement" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Snapshot" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="State Map" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Output plots (trans)" sheetId="12" state="visible" r:id="rId13"/>
@@ -694,12 +694,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\ MMM\ YYYY"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="167" formatCode="0.00%"/>
-    <numFmt numFmtId="168" formatCode="&quot;WAAR&quot;;&quot;WAAR&quot;;&quot;ONWAAR&quot;"/>
+    <numFmt numFmtId="166" formatCode="&quot;WAAR&quot;;&quot;WAAR&quot;;&quot;ONWAAR&quot;"/>
+    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="168" formatCode="0.00%"/>
+    <numFmt numFmtId="169" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -918,11 +919,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -934,7 +935,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -942,15 +943,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -962,31 +963,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="168" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1002,7 +1003,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1010,7 +1011,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1022,7 +1023,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1038,19 +1039,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1158,7 +1159,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.21"/>
@@ -1306,7 +1307,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.27"/>
@@ -1508,11 +1509,11 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.21875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="8.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,7 +1680,7 @@
       <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.33"/>
@@ -1962,7 +1963,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.96"/>
@@ -1974,7 +1975,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.4"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="11" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,11 +2628,10 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="20.83"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="2" style="41" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20775,16 +20774,16 @@
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="6" style="1" width="8.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="6" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21308,14 +21307,14 @@
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="11" width="11.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="11" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21536,11 +21535,11 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="11.52"/>
@@ -21805,7 +21804,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.6"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="1" width="11.52"/>
@@ -22021,17 +22020,17 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="8.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1006" min="12" style="1" width="8.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1011" min="1007" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1012" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1006" min="12" style="1" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1011" min="1007" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1012" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22910,6 +22909,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="10">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:B13 G11:G13 L11:L13" type="list">
+      <formula1>Misc!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B17 G17 L17 B25 G25 L25" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -22932,10 +22935,6 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9:B10 G9:G10 L9:L10" type="decimal">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:B13 G11:G13 L11:L13" type="list">
-      <formula1>Misc!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B14 G14 L14" type="decimal">
@@ -22976,7 +22975,7 @@
       <selection pane="bottomRight" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="17.4"/>
@@ -23864,12 +23863,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="17">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C7 B11:C11 B15:C15 B19:C19 B23:C23 B27:C27" type="list">
+      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C7 B11:C11 B15:C15 B19:C19 B23:C23 B27:C27" type="list">
-      <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:H6 A8:C8 G8:G10 A9 C9 H10 A12:C12 G12:G14 A13 C13 H14 A16:C16 G16:G18 A17 C17 H18 A20:C20 G20:G22 A21 C21 H22 A24:C24 G24:G26 A25 C25 H26 A28:C28 G28:G29 A29 C29" type="none">
@@ -23958,7 +23957,7 @@
       <selection pane="bottomRight" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.37"/>
@@ -29889,14 +29888,14 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="1" width="8.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="1" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added initial population plots/reports (v0.6.0)
* Added the functions that allow generation of composition and age reports and plots of the initial population of the simulation.
* Added code to request these from Excel.
* Added some unit tests for these functions.
</commit_message>
<xml_diff>
--- a/test/base/baseConfig.xlsx
+++ b/test/base/baseConfig.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="209">
   <si>
     <t xml:space="preserve">General simulation parameters</t>
   </si>
@@ -447,25 +447,49 @@
     <t xml:space="preserve">Snapshot file</t>
   </si>
   <si>
-    <t xml:space="preserve">photo</t>
+    <t xml:space="preserve">test foto 1</t>
   </si>
   <si>
-    <t xml:space="preserve">ID column number</t>
+    <t xml:space="preserve">Snapshot sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">Tenure info column number</t>
+    <t xml:space="preserve">Sheet1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tenure info column</t>
   </si>
   <si>
     <t xml:space="preserve">Is recruitment date?</t>
   </si>
   <si>
-    <t xml:space="preserve">Age info column number</t>
+    <t xml:space="preserve">Age info column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
   </si>
   <si>
     <t xml:space="preserve">Is birth date?</t>
   </si>
   <si>
-    <t xml:space="preserve">Last transition time column number</t>
+    <t xml:space="preserve">Last transition time column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current node column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate attributes/nodes?</t>
   </si>
   <si>
     <t xml:space="preserve">Max columns to import</t>
@@ -477,16 +501,13 @@
     <t xml:space="preserve">Col nrs to import</t>
   </si>
   <si>
-    <t xml:space="preserve">Seniority</t>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">Branch</t>
+    <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">Language</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
+    <t xml:space="preserve">D</t>
   </si>
   <si>
     <t xml:space="preserve">Plot of State Network</t>
@@ -697,7 +718,7 @@
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\ MMM\ YYYY"/>
-    <numFmt numFmtId="166" formatCode="&quot;WAAR&quot;;&quot;WAAR&quot;;&quot;ONWAAR&quot;"/>
+    <numFmt numFmtId="166" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
     <numFmt numFmtId="167" formatCode="General"/>
     <numFmt numFmtId="168" formatCode="0.00%"/>
     <numFmt numFmtId="169" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
@@ -1268,12 +1289,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="4">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11 B14" type="list">
       <formula1>Misc!$B$1:$B$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9" type="whole">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="whole">
@@ -1301,10 +1322,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1327,7 +1348,7 @@
         <v>119</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,73 +1363,72 @@
       <c r="A5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>1</v>
+      <c r="B5" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>7</v>
+      <c r="A6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>15</v>
+        <v>126</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="4" t="n">
-        <v>6</v>
+        <v>127</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>8</v>
-      </c>
-    </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12" s="12" t="n">
-        <v>100</v>
-      </c>
-      <c r="C12" s="13" t="str">
-        <f aca="false">IF(B12=B13,"Increase Max columns to import","")</f>
-        <v/>
+      <c r="A12" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" s="14" t="n">
-        <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B13,3,-1,B12)),0,0),0)-1,B12)</f>
-        <v>4</v>
+      <c r="A13" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,74 +1437,151 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>51</v>
+        <v>136</v>
+      </c>
+      <c r="B15" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="C15" s="13" t="str">
+        <f aca="false">IF(B15=B16,"Increase Max columns to import","")</f>
+        <v/>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>131</v>
+      <c r="A16" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" s="14" t="n">
+        <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B16,3,-1,B15)),0,0),0)-1,B15)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>132</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>133</v>
+      <c r="A18" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>134</v>
+      <c r="A19" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
-  <conditionalFormatting sqref="A4:B4">
+  <conditionalFormatting sqref="A4:B5">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>Snapshot!$B$3="NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B9" type="list">
+  <dataValidations count="4">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B8 B10 B13" type="list">
       <formula1>Misc!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B6 B8 B10" type="whole">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B15" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B12" type="whole">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6:B7 B9 B11:B12" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A16:A20" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A19:A48" type="none">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B16:B20" type="list">
-      <formula1>INDEX(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2),SMALL(IF(ISTEXT(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2)),ROW(OFFSET(Attributes!$A$7,0,0,Attributes!$B$4*3-2))-ROW(Attributes!$A$6),""),ROW(INDIRECT("1:"&amp;Attributes!$B$4))))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1518,7 +1615,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -1528,7 +1625,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>12</v>
@@ -1536,7 +1633,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>25</v>
@@ -1544,7 +1641,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>12</v>
@@ -1552,10 +1649,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,7 +1661,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B8" s="12" t="n">
         <v>1000</v>
@@ -1576,7 +1673,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B9" s="17" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B9,2,0,B8)),0,0),0)-1,B8)</f>
@@ -1589,25 +1686,25 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,7 +1792,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B1" s="40"/>
     </row>
@@ -1705,7 +1802,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>12</v>
@@ -1713,7 +1810,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>12</v>
@@ -1721,7 +1818,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>12</v>
@@ -1729,10 +1826,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1741,7 +1838,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B8" s="12" t="n">
         <v>50</v>
@@ -1753,7 +1850,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B9" s="14" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B9,3,3,B8)),0,0),0)-1,B8)</f>
@@ -1766,19 +1863,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1787,10 +1884,10 @@
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E12" s="18"/>
     </row>
@@ -1800,10 +1897,10 @@
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E13" s="18"/>
     </row>
@@ -1813,7 +1910,7 @@
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>42</v>
@@ -1826,7 +1923,7 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>42</v>
@@ -1839,7 +1936,7 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="18"/>
@@ -1850,7 +1947,7 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="18"/>
@@ -1861,7 +1958,7 @@
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="18"/>
@@ -1872,7 +1969,7 @@
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="18"/>
@@ -1979,7 +2076,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B1" s="40"/>
     </row>
@@ -1989,7 +2086,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>12</v>
@@ -1997,7 +2094,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>12</v>
@@ -2005,7 +2102,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>12</v>
@@ -2013,10 +2110,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,7 +2122,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B8" s="12" t="n">
         <v>50</v>
@@ -2037,7 +2134,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B9" s="14" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B9,4,0,B8)),0,0),0)-1,B8)</f>
@@ -2062,32 +2159,32 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="15" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,7 +2214,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="36" t="s">
@@ -2144,7 +2241,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="36" t="s">
@@ -2171,7 +2268,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="36" t="s">
@@ -2198,7 +2295,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="36" t="s">
@@ -2225,7 +2322,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="36" t="s">
@@ -2252,7 +2349,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="36" t="s">
@@ -2279,7 +2376,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="36" t="s">
@@ -2306,7 +2403,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="36" t="s">
@@ -2333,7 +2430,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="36" t="s">
@@ -2387,7 +2484,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="36" t="s">
@@ -2441,7 +2538,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="36" t="s">
@@ -2468,7 +2565,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="36" t="s">
@@ -2495,7 +2592,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="36" t="s">
@@ -2522,7 +2619,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="36" t="s">
@@ -2549,7 +2646,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="36" t="s">
@@ -2643,19 +2740,19 @@
         <v>15</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D1" s="41" t="s">
         <v>85</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="H1" s="41" t="n">
         <f aca="false">ROWS(H2:H1001)-COUNTIF(H2:H1001,"")</f>
@@ -2670,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="41" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,16 +2779,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>110</v>
@@ -2719,16 +2816,16 @@
         <v>.</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>79</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="G3" s="41" t="s">
         <v>106</v>
@@ -2756,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E4" s="41" t="s">
         <v>25</v>
@@ -2784,7 +2881,7 @@
         <v>'catalogue.xlsx'#'General'.</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="H5" s="43" t="str">
         <f aca="true" t="array" ref="H5:H5">IFERROR(INDEX(OFFSET('Transition types'!$A$6,1,0,'Transition types'!$B$4),SMALL(IF(OFFSET('Transition types'!$C$6,1,0,'Transition types'!$B$4)="IN",OFFSET($K$2,0,0,'Transition types'!$B$4)),ROWS($K$2:$K5))),"")</f>
@@ -2809,7 +2906,7 @@
         <v>'catalogue.xlsx'#'Attributes'.</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H6" s="43" t="str">
         <f aca="true" t="array" ref="H6:H6">IFERROR(INDEX(OFFSET('Transition types'!$A$6,1,0,'Transition types'!$B$4),SMALL(IF(OFFSET('Transition types'!$C$6,1,0,'Transition types'!$B$4)="IN",OFFSET($K$2,0,0,'Transition types'!$B$4)),ROWS($K$2:$K6))),"")</f>
@@ -2834,7 +2931,7 @@
         <v>'catalogue.xlsx'#'States'.</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="H7" s="43" t="str">
         <f aca="true" t="array" ref="H7:H7">IFERROR(INDEX(OFFSET('Transition types'!$A$6,1,0,'Transition types'!$B$4),SMALL(IF(OFFSET('Transition types'!$C$6,1,0,'Transition types'!$B$4)="IN",OFFSET($K$2,0,0,'Transition types'!$B$4)),ROWS($K$2:$K7))),"")</f>
@@ -23863,12 +23960,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="17">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C7 B11:C11 B15:C15 B19:C19 B23:C23 B27:C27" type="list">
       <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:H6 A8:C8 G8:G10 A9 C9 H10 A12:C12 G12:G14 A13 C13 H14 A16:C16 G16:G18 A17 C17 H18 A20:C20 G20:G22 A21 C21 H22 A24:C24 G24:G26 A25 C25 H26 A28:C28 G28:G29 A29 C29" type="none">
@@ -29810,12 +29907,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="15">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7" type="list">
       <formula1>OFFSET('Base Nodes'!$A$7,0,0,'Base Nodes'!$B$4)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11 B15 B19 B23 B27" type="list">
@@ -29888,7 +29985,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>